<commit_message>
Fucking ready more then evevr lets start and finish this phase in my  Ph.D
</commit_message>
<xml_diff>
--- a/ipa_2/myUtils/instructions.xlsx
+++ b/ipa_2/myUtils/instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_2\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4569FD-7DA5-4B42-A075-4919E636E0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F687CE9-26BE-4EF0-AC43-7684C6A1F09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="302" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="302" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>השלב הבא</t>
   </si>
   <si>
-    <t>כעת, לצורך הדוגמה, אתה יכול לבחור בין {} , לבין {} וכך גם האדם השני. כל אחד מכם בוחר לפי ראות עיניו, ומתוך הניסיון להגיע לתוצאה הטובה ביותר עבורו. אתה יכול לבחור או בשורה הראשונה ({}) או בשורה השניה ({}). כך גם האדם השני יכול לבחור בין הטור הימני לשמאלי. בכל צירוף של שתי בחירות רשום כמה אתה תקבל וכמה האחר. התוצאה שלך רשומה תמיד מצד שמאל. לצורך בדיקת הבנה - בחר כעת את השורה התחונה - {}.</t>
-  </si>
-  <si>
     <t>יפה מאוד! כאשר אתה לוחץ על אחת השורות, זה אומר שבחרת באפשרות הזו. כמה שתקבל תלוי במה יבחר האדם השני. בזמן שאתה מבצע את בחירתך אינך יכול לראות מה האדם השני בחר, אך גם כשאר השחקן השני בוחר, אתה לא יכול לראות את הבחירה שלו. התוצאות יקבעו רק לאחר מכן. בוא נמשיך בלמידה - לחץ עכשיו על האופציה העליונה.</t>
   </si>
   <si>
@@ -446,6 +443,9 @@
   </si>
   <si>
     <t>את בחרת, אם המשתתף האחר יבחר, את תקבלי, והאחר יקבל, ואם המשתתף אחר יבחר</t>
+  </si>
+  <si>
+    <t>כעת, לצורך הדוגמה, אתה יכול לבחור בין {} , לבין {} וכך גם האדם השני. כל אחד מכם בוחר לפי ראות עיניו, ומתוך הניסיון להגיע לתוצאה הטובה ביותר עבורו. אתה יכול לבחור או בשורה הראשונה ({}) או בשורה השניה ({}). כך גם האדם השני יכול לבחור בין הטור הימני לשמאלי. בכל צירוף של שתי בחירות רשום כמה אתה תקבל וכמה האחר. התוצאות האפשריות שלך רשומות תמיד מצד שמאל בכל תא, והן יופיעו בצבע סגול, התוצאות האפשריות של האחר תמיד יופיעו מצד ימין בכל תא והן יופיעו בצבע כתום. לצורך בדיקת הבנה - בחר כעת את השורה התחונה - {}.</t>
   </si>
 </sst>
 </file>
@@ -808,20 +808,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="C39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="48.44140625" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
@@ -888,7 +888,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
@@ -910,7 +910,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
@@ -954,7 +954,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>47</v>
       </c>
@@ -976,7 +976,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
@@ -998,7 +998,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
@@ -1020,7 +1020,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1042,7 +1042,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1050,20 +1050,20 @@
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1084,7 +1084,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>1</v>
       </c>
@@ -1147,7 +1147,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>1</v>
       </c>
@@ -1168,7 +1168,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>1</v>
       </c>
@@ -1189,7 +1189,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>2</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>3</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>3</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -1304,20 +1304,20 @@
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>9</v>
       </c>
@@ -1325,20 +1325,20 @@
         <v>8</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>4</v>
       </c>
@@ -1367,19 +1367,19 @@
         <v>8</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
@@ -1387,20 +1387,20 @@
         <v>8</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>5</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>5</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>5</v>
       </c>
@@ -1463,7 +1463,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -1471,20 +1471,20 @@
         <v>42</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
@@ -1505,7 +1505,7 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>5</v>
       </c>
@@ -1513,20 +1513,20 @@
         <v>82</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>5</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
@@ -1568,7 +1568,7 @@
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>29</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>27</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>27</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>27</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1648,16 +1648,16 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" t="s">
         <v>105</v>
       </c>
-      <c r="D40" t="s">
-        <v>105</v>
-      </c>
-      <c r="E40" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -1665,16 +1665,16 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -1682,16 +1682,16 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -1699,16 +1699,16 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -1716,16 +1716,16 @@
         <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E44" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -1733,16 +1733,16 @@
         <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E45" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -1818,7 +1818,7 @@
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -1826,13 +1826,13 @@
         <v>82</v>
       </c>
       <c r="C50" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>